<commit_message>
Functies en OF gemaakt
</commit_message>
<xml_diff>
--- a/NetworkScheduling/Assignment 1/Input_Ass1P1.xlsx
+++ b/NetworkScheduling/Assignment 1/Input_Ass1P1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blopesdossanto/Documents/01 TU Delft/02 Education/02 Courses/2017:2018/AE4424 Network Scheduling/Assignments/Assignment 1/Assignment 1a/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\AirlinePlanning\NetworkScheduling\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB65198-A96F-498F-9DFD-BC70C0B3098D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="-21140" windowWidth="16320" windowHeight="16540"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcs" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Arc</t>
   </si>
@@ -46,54 +47,6 @@
     <t>Capacity</t>
   </si>
   <si>
-    <t>ANC</t>
-  </si>
-  <si>
-    <t>CVG</t>
-  </si>
-  <si>
-    <t>LAX</t>
-  </si>
-  <si>
-    <t>ICN</t>
-  </si>
-  <si>
-    <t>PVG</t>
-  </si>
-  <si>
-    <t>HKG</t>
-  </si>
-  <si>
-    <t>LEJ</t>
-  </si>
-  <si>
-    <t>EMA</t>
-  </si>
-  <si>
-    <t>JFK</t>
-  </si>
-  <si>
-    <t>BAH</t>
-  </si>
-  <si>
-    <t>BRU</t>
-  </si>
-  <si>
-    <t>LOS</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>DXB</t>
-  </si>
-  <si>
-    <t>BKK</t>
-  </si>
-  <si>
-    <t>SIN</t>
-  </si>
-  <si>
     <t>Commodity</t>
   </si>
   <si>
@@ -103,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -461,16 +414,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,15 +440,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -504,15 +457,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>7</v>
@@ -521,15 +474,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>15</v>
@@ -538,15 +491,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>13</v>
@@ -555,15 +508,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>18</v>
@@ -572,15 +525,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
       </c>
       <c r="D7" s="1">
         <v>12</v>
@@ -589,15 +542,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
       </c>
       <c r="D8" s="1">
         <v>20</v>
@@ -606,15 +559,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12</v>
       </c>
       <c r="D9" s="1">
         <v>17</v>
@@ -623,15 +576,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <v>15</v>
@@ -640,15 +593,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
       </c>
       <c r="D11" s="1">
         <v>19</v>
@@ -657,15 +610,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <v>17</v>
@@ -674,15 +627,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
@@ -691,15 +644,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
+      <c r="B14" s="2">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>10</v>
@@ -708,15 +661,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>4</v>
@@ -725,15 +678,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13</v>
       </c>
       <c r="D16" s="1">
         <v>9</v>
@@ -742,15 +695,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
+      <c r="B17" s="1">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>10</v>
@@ -759,15 +712,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5</v>
       </c>
       <c r="D18" s="1">
         <v>13</v>
@@ -776,15 +729,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
+      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
       </c>
       <c r="D19" s="1">
         <v>22</v>
@@ -793,15 +746,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
+        <v>8</v>
       </c>
       <c r="D20" s="1">
         <v>25</v>
@@ -810,15 +763,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>18</v>
+      <c r="B21" s="1">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6</v>
       </c>
       <c r="D21" s="1">
         <v>8</v>
@@ -827,15 +780,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>14</v>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>12</v>
@@ -844,15 +797,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
         <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D23" s="1">
         <v>11</v>
@@ -861,15 +814,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8</v>
       </c>
       <c r="D24" s="1">
         <v>13</v>
@@ -878,15 +831,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>19</v>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
       </c>
       <c r="D25" s="1">
         <v>12</v>
@@ -895,15 +848,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>15</v>
       </c>
       <c r="D26" s="1">
         <v>9</v>
@@ -912,15 +865,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>10</v>
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8</v>
       </c>
       <c r="D27" s="1">
         <v>10</v>
@@ -929,15 +882,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>20</v>
+      <c r="B28" s="1">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>15</v>
       </c>
       <c r="D28" s="1">
         <v>6</v>
@@ -946,15 +899,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>20</v>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>15</v>
       </c>
       <c r="D29" s="1">
         <v>3</v>
@@ -963,15 +916,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>10</v>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1">
+        <v>8</v>
       </c>
       <c r="D30" s="1">
         <v>5</v>
@@ -980,15 +933,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1">
         <v>9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>14</v>
       </c>
       <c r="D31" s="1">
         <v>4</v>
@@ -1003,18 +956,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1023,570 +976,573 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
+      <c r="B9" s="1">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
+      <c r="B17" s="1">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>14</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
+      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>13</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>11</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>19</v>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
+      <c r="B23" s="1">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
+      <c r="B24" s="1">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="1">
         <v>6</v>
       </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>7</v>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>11</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
+      <c r="B28" s="1">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10</v>
       </c>
       <c r="D28" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>9</v>
+      <c r="B29" s="1">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>14</v>
       </c>
       <c r="D29" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1">
+        <v>12</v>
       </c>
       <c r="D30" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>18</v>
+      <c r="B31" s="1">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>6</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>16</v>
+      <c r="B32" s="1">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1">
+        <v>13</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
+      <c r="B33" s="1">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
       </c>
       <c r="D33" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>13</v>
+      <c r="B34" s="1">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1">
+        <v>10</v>
       </c>
       <c r="D34" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>15</v>
+      <c r="B35" s="1">
+        <v>14</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>6</v>
+      <c r="B36" s="1">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
       </c>
       <c r="D36" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>8</v>
+      <c r="B37" s="1">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1">
+        <v>9</v>
       </c>
       <c r="D37" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>12</v>
+      <c r="B38" s="1">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1">
+        <v>7</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>12</v>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>7</v>
       </c>
       <c r="D39" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>11</v>
       </c>
       <c r="D40" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>16</v>
+      <c r="B41" s="1">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1">
+        <v>13</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>